<commit_message>
update of the GL results
</commit_message>
<xml_diff>
--- a/single_digit/Results/NEW/3vs5_SVM_GL_20training.xlsx
+++ b/single_digit/Results/NEW/3vs5_SVM_GL_20training.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Group_Learning\single_digit\Results\NEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0BDB7-9D31-40CB-885B-A6B505BDEF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7658E-A36C-4F0B-8953-26CD68F62709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{60F57292-22A5-4A33-BAC1-D93E5267D72A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>SVM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +73,10 @@
   </si>
   <si>
     <t>Task: 3 vs 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2817,10 +2821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D86EA0-3C88-40C3-A1C5-042D836277E7}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -2974,6 +2978,16 @@
       <c r="B23">
         <f>AVERAGE(B3:B22)</f>
         <v>0.124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <f>STDEV(A3:A12)</f>
+        <v>2.4152294576982401E-2</v>
+      </c>
+      <c r="B24">
+        <f>STDEV(B3:B12)</f>
+        <v>3.5103022978402031E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3474,8 +3488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E7B3FA-A786-498B-86FF-4C69BB3470EF}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -3700,9 +3714,29 @@
         <v>3.0000000000000006E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>6</v>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <f>STDEV(B3:B12)</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:F24" si="1">STDEV(C3:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1.5811388300841896E-2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2.10818510677892E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>5.3748384988657E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3905,23 +3939,23 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:F48" si="1">AVERAGE(B28:B47)</f>
+        <f t="shared" ref="B48:F48" si="2">AVERAGE(B28:B47)</f>
         <v>0.11900000000000002</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.10450000000000001</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1065</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12050000000000001</v>
       </c>
     </row>
@@ -3930,23 +3964,23 @@
         <v>6</v>
       </c>
       <c r="B49">
-        <f t="shared" ref="B49:F49" si="2">STDEVA(B28:B47)</f>
+        <f t="shared" ref="B49:F49" si="3">STDEVA(B28:B47)</f>
         <v>4.6654760385909821E-2</v>
       </c>
       <c r="C49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3120151636797227E-2</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.145102012124041E-2</v>
       </c>
       <c r="E49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7919573407620827E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9102309950319094E-2</v>
       </c>
     </row>

</xml_diff>